<commit_message>
Eroski still need scraping non per kg/l products and BM can't be pooled as request_html does not work with multiprocessing
</commit_message>
<xml_diff>
--- a/LIBRO-BASE-PRODUCTOS_ok.xlsx
+++ b/LIBRO-BASE-PRODUCTOS_ok.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\110414\PycharmProjects\Seguidor-de-precios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DD36B1-0327-4523-9845-C6C86F267517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC6C676-58F1-4558-85E1-8EEFFD1A7679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1228,7 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1255,6 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1542,8 +1543,8 @@
   <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,7 +1587,7 @@
       <c r="D2" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="18" t="s">
         <v>259</v>
       </c>
       <c r="F2" s="2"/>
@@ -1666,7 +1667,7 @@
       <c r="D7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="12" t="s">
         <v>264</v>
       </c>
       <c r="F7" s="1"/>
@@ -2192,7 +2193,7 @@
       <c r="D41" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="12" t="s">
         <v>292</v>
       </c>
       <c r="F41" s="1"/>
@@ -2269,10 +2270,10 @@
         <v>18</v>
       </c>
       <c r="C46" s="6"/>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" s="12" t="s">
         <v>298</v>
       </c>
       <c r="F46" s="1"/>
@@ -2597,10 +2598,10 @@
         <v>49</v>
       </c>
       <c r="C67" s="6"/>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" s="12" t="s">
         <v>316</v>
       </c>
       <c r="F67" s="1"/>
@@ -2769,10 +2770,10 @@
         <v>76</v>
       </c>
       <c r="C78" s="6"/>
-      <c r="D78" s="1" t="s">
+      <c r="D78" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" s="12" t="s">
         <v>326</v>
       </c>
       <c r="F78" s="1"/>
@@ -3536,8 +3537,17 @@
     <hyperlink ref="E48" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="D85" r:id="rId6" xr:uid="{86F9444C-0ADF-40D0-B4A1-4101034FA3BE}"/>
     <hyperlink ref="D83" r:id="rId7" xr:uid="{CCAD6A6E-05CE-470F-BBE8-3C736867E146}"/>
+    <hyperlink ref="E2" r:id="rId8" xr:uid="{5A2A8BB7-36C5-48F5-88F2-20EEFA2B806F}"/>
+    <hyperlink ref="D46" r:id="rId9" xr:uid="{CD958F7D-5BE0-4C7F-839E-2951984CFC19}"/>
+    <hyperlink ref="E46" r:id="rId10" xr:uid="{7A8AEA08-B6C8-41EC-9D0A-B07A5E6D36C3}"/>
+    <hyperlink ref="D67" r:id="rId11" xr:uid="{60DF1E27-DF5B-4CCE-B901-ACB6E45CA5ED}"/>
+    <hyperlink ref="E67" r:id="rId12" xr:uid="{DE02EE3E-B04E-4DF3-9195-9A180D4B6E5A}"/>
+    <hyperlink ref="D78" r:id="rId13" xr:uid="{B7CB9223-62E7-44A8-A27C-EB6FF721AA2B}"/>
+    <hyperlink ref="E78" r:id="rId14" xr:uid="{E16B507F-4689-48B7-B05A-51C5E0FB6A02}"/>
+    <hyperlink ref="E7" r:id="rId15" xr:uid="{470A72BA-2F1A-42F3-93C9-AED4221D3F89}"/>
+    <hyperlink ref="E41" r:id="rId16" xr:uid="{ECA7933E-8759-4F44-8D52-FE953633F48A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>